<commit_message>
Agregado chequeo de administrador
</commit_message>
<xml_diff>
--- a/4.-Documentación/Diagrama de Gantt previsto.xlsx
+++ b/4.-Documentación/Diagrama de Gantt previsto.xlsx
@@ -5,28 +5,35 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\mega\2.-CursosyApuntes\DesarrollodeAplicacionesMultiplataforma\1.-Proyectofinalmodulo\4.-Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VehicleGest\4.-Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B12351-44AC-4F30-8B6C-547A0A2E72EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98277F7-5069-438B-9802-AE1B01BC77FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diagrama previsión" sheetId="11" r:id="rId1"/>
     <sheet name="Diagrama real" sheetId="16" r:id="rId2"/>
+    <sheet name="Diagrama ampliación" sheetId="18" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">'Diagrama ampliación'!$1:$17</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Diagrama previsión'!$1:$71</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Diagrama real'!$1:$71</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Diagrama real'!$1:$73</definedName>
+    <definedName name="task_end" localSheetId="2">'Diagrama ampliación'!$E1</definedName>
     <definedName name="task_end" localSheetId="0">'Diagrama previsión'!$E1</definedName>
     <definedName name="task_end" localSheetId="1">'Diagrama real'!$E1</definedName>
+    <definedName name="task_progress" localSheetId="2">'Diagrama ampliación'!$C1</definedName>
     <definedName name="task_progress" localSheetId="0">'Diagrama previsión'!$C1</definedName>
     <definedName name="task_progress" localSheetId="1">'Diagrama real'!$C1</definedName>
+    <definedName name="task_start" localSheetId="2">'Diagrama ampliación'!$D1</definedName>
     <definedName name="task_start" localSheetId="0">'Diagrama previsión'!$D1</definedName>
     <definedName name="task_start" localSheetId="1">'Diagrama real'!$D1</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="2">'Diagrama ampliación'!$4:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Diagrama previsión'!$4:$6</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Diagrama real'!$4:$6</definedName>
+    <definedName name="today" localSheetId="2">'Diagrama ampliación'!$D$3</definedName>
     <definedName name="today" localSheetId="0">'Diagrama previsión'!$D$3</definedName>
     <definedName name="today" localSheetId="1">'Diagrama real'!$D$3</definedName>
     <definedName name="valuevx">42.314159</definedName>
@@ -117,8 +124,42 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Vertex42.com Templates</author>
+  </authors>
+  <commentList>
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{C5305B05-5110-4946-B226-B0B6188734BA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DAYS:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This column calculates the duration of the task in calendar days. The duration includes both the Start and End dates.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="88">
   <si>
     <t>SIMPLE GANTT CHART by Vertex42.com</t>
   </si>
@@ -349,6 +390,39 @@
   </si>
   <si>
     <t>Listado de alertas</t>
+  </si>
+  <si>
+    <t>Creación de ITVs</t>
+  </si>
+  <si>
+    <t>Detalle de ITVs</t>
+  </si>
+  <si>
+    <t>Edición de ITVs</t>
+  </si>
+  <si>
+    <t>Eliminación de ITVs</t>
+  </si>
+  <si>
+    <t>Creación de alertas</t>
+  </si>
+  <si>
+    <t>Edición de alertas</t>
+  </si>
+  <si>
+    <t>Vehículos asignados por empleado</t>
+  </si>
+  <si>
+    <t>Servicios asignados por empleado</t>
+  </si>
+  <si>
+    <t>Recodificación completa</t>
+  </si>
+  <si>
+    <t>Revisión de la memoria</t>
+  </si>
+  <si>
+    <t>Realización del video</t>
   </si>
 </sst>
 </file>
@@ -752,7 +826,7 @@
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -994,11 +1068,11 @@
     <xf numFmtId="0" fontId="3" fillId="18" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -1009,11 +1083,17 @@
     <xf numFmtId="165" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1021,7 +1101,37 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="57">
+  <dxfs count="60">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -1598,15 +1708,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="wholeTable" dxfId="56"/>
-      <tableStyleElement type="headerRow" dxfId="55"/>
-      <tableStyleElement type="totalRow" dxfId="54"/>
-      <tableStyleElement type="firstColumn" dxfId="53"/>
-      <tableStyleElement type="lastColumn" dxfId="52"/>
-      <tableStyleElement type="firstRowStripe" dxfId="51"/>
-      <tableStyleElement type="secondRowStripe" dxfId="50"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="49"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="48"/>
+      <tableStyleElement type="wholeTable" dxfId="59"/>
+      <tableStyleElement type="headerRow" dxfId="58"/>
+      <tableStyleElement type="totalRow" dxfId="57"/>
+      <tableStyleElement type="firstColumn" dxfId="56"/>
+      <tableStyleElement type="lastColumn" dxfId="55"/>
+      <tableStyleElement type="firstRowStripe" dxfId="54"/>
+      <tableStyleElement type="secondRowStripe" dxfId="53"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="52"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="51"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1994,24 +2104,24 @@
       <c r="E1" s="48"/>
       <c r="F1" s="1"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="90"/>
-      <c r="O1" s="90"/>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="90"/>
-      <c r="S1" s="90"/>
-      <c r="T1" s="90"/>
-      <c r="U1" s="90"/>
-      <c r="V1" s="90"/>
-      <c r="W1" s="90"/>
-      <c r="X1" s="90"/>
-      <c r="Y1" s="90"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
+      <c r="U1" s="86"/>
+      <c r="V1" s="86"/>
+      <c r="W1" s="86"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="86"/>
     </row>
     <row r="2" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
@@ -2020,10 +2130,10 @@
       <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="85">
+      <c r="D2" s="90">
         <v>44854</v>
       </c>
-      <c r="E2" s="86"/>
+      <c r="E2" s="91"/>
     </row>
     <row r="3" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
@@ -2032,10 +2142,10 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="85">
+      <c r="D3" s="90">
         <v>44900</v>
       </c>
-      <c r="E3" s="86"/>
+      <c r="E3" s="91"/>
     </row>
     <row r="4" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
@@ -7470,17 +7580,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="H1:Y1"/>
-    <mergeCell ref="AI4:AO4"/>
-    <mergeCell ref="AP4:AV4"/>
-    <mergeCell ref="AW4:BC4"/>
-    <mergeCell ref="BD4:BJ4"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="G4:M4"/>
     <mergeCell ref="N4:T4"/>
     <mergeCell ref="U4:AA4"/>
     <mergeCell ref="AB4:AH4"/>
     <mergeCell ref="D3:E3"/>
+    <mergeCell ref="H1:Y1"/>
+    <mergeCell ref="AI4:AO4"/>
+    <mergeCell ref="AP4:AV4"/>
+    <mergeCell ref="AW4:BC4"/>
+    <mergeCell ref="BD4:BJ4"/>
   </mergeCells>
   <conditionalFormatting sqref="C7:C18 C20:C24 C26:C31 C38 C41:C44 C46:C49 C52:C71 C33:C36">
     <cfRule type="dataBar" priority="68">
@@ -7497,15 +7607,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:BJ31 G38:BJ38 G41:BJ44 G46:BJ49 G52:BJ71 G33:BJ36">
-    <cfRule type="expression" dxfId="47" priority="81">
+    <cfRule type="expression" dxfId="50" priority="81">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="82" stopIfTrue="1">
       <formula>AND(task_end&gt;=G$5,task_start&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:BJ31 G38:BJ38 G41:BJ44 G46:BJ49 G52:BJ71 G33:BJ36">
-    <cfRule type="expression" dxfId="45" priority="83">
+    <cfRule type="expression" dxfId="48" priority="83">
       <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7566,28 +7676,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:BJ32">
-    <cfRule type="expression" dxfId="44" priority="42">
+    <cfRule type="expression" dxfId="47" priority="42">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="43" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="43" stopIfTrue="1">
       <formula>AND(task_end&gt;=G$5,task_start&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:BJ32">
-    <cfRule type="expression" dxfId="42" priority="44">
+    <cfRule type="expression" dxfId="45" priority="44">
       <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39:BJ39">
-    <cfRule type="expression" dxfId="41" priority="38">
+    <cfRule type="expression" dxfId="44" priority="38">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="39" stopIfTrue="1">
+    <cfRule type="expression" dxfId="43" priority="39" stopIfTrue="1">
       <formula>AND(task_end&gt;=G$5,task_start&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39:BJ39">
-    <cfRule type="expression" dxfId="39" priority="40">
+    <cfRule type="expression" dxfId="42" priority="40">
       <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7606,15 +7716,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37:BJ37">
-    <cfRule type="expression" dxfId="38" priority="22">
+    <cfRule type="expression" dxfId="41" priority="22">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="23" stopIfTrue="1">
       <formula>AND(task_end&gt;=G$5,task_start&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37:BJ37">
-    <cfRule type="expression" dxfId="36" priority="24">
+    <cfRule type="expression" dxfId="39" priority="24">
       <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7633,15 +7743,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40:BJ40">
-    <cfRule type="expression" dxfId="35" priority="18">
+    <cfRule type="expression" dxfId="38" priority="18">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="19" stopIfTrue="1">
       <formula>AND(task_end&gt;=G$5,task_start&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40:BJ40">
-    <cfRule type="expression" dxfId="33" priority="20">
+    <cfRule type="expression" dxfId="36" priority="20">
       <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7660,15 +7770,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45:BJ45">
-    <cfRule type="expression" dxfId="32" priority="14">
+    <cfRule type="expression" dxfId="35" priority="14">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="15" stopIfTrue="1">
       <formula>AND(task_end&gt;=G$5,task_start&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45:BJ45">
-    <cfRule type="expression" dxfId="30" priority="16">
+    <cfRule type="expression" dxfId="33" priority="16">
       <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7687,15 +7797,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50:BJ50">
-    <cfRule type="expression" dxfId="29" priority="6">
+    <cfRule type="expression" dxfId="32" priority="6">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="7" stopIfTrue="1">
       <formula>AND(task_end&gt;=G$5,task_start&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50:BJ50">
-    <cfRule type="expression" dxfId="27" priority="8">
+    <cfRule type="expression" dxfId="30" priority="8">
       <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7714,15 +7824,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51:BJ51">
-    <cfRule type="expression" dxfId="26" priority="2">
+    <cfRule type="expression" dxfId="29" priority="2">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="3" stopIfTrue="1">
       <formula>AND(task_end&gt;=G$5,task_start&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51:BJ51">
-    <cfRule type="expression" dxfId="24" priority="4">
+    <cfRule type="expression" dxfId="27" priority="4">
       <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7903,11 +8013,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BJ75"/>
+  <dimension ref="A1:BJ77"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:BJ60"/>
+    <sheetView showGridLines="0" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="BJ76" sqref="BJ76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7930,24 +8040,24 @@
       <c r="E1" s="48"/>
       <c r="F1" s="46"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="90"/>
-      <c r="I1" s="90"/>
-      <c r="J1" s="90"/>
-      <c r="K1" s="90"/>
-      <c r="L1" s="90"/>
-      <c r="M1" s="90"/>
-      <c r="N1" s="90"/>
-      <c r="O1" s="90"/>
-      <c r="P1" s="90"/>
-      <c r="Q1" s="90"/>
-      <c r="R1" s="90"/>
-      <c r="S1" s="90"/>
-      <c r="T1" s="90"/>
-      <c r="U1" s="90"/>
-      <c r="V1" s="90"/>
-      <c r="W1" s="90"/>
-      <c r="X1" s="90"/>
-      <c r="Y1" s="90"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
+      <c r="U1" s="86"/>
+      <c r="V1" s="86"/>
+      <c r="W1" s="86"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="86"/>
     </row>
     <row r="2" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
@@ -7956,10 +8066,10 @@
       <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="85">
+      <c r="D2" s="90">
         <v>44854</v>
       </c>
-      <c r="E2" s="86"/>
+      <c r="E2" s="91"/>
     </row>
     <row r="3" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="8" t="s">
@@ -7968,10 +8078,10 @@
       <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="85">
+      <c r="D3" s="90">
         <v>44900</v>
       </c>
-      <c r="E3" s="86"/>
+      <c r="E3" s="91"/>
     </row>
     <row r="4" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="5" t="s">
@@ -8537,7 +8647,7 @@
       <c r="D7" s="20"/>
       <c r="E7" s="21"/>
       <c r="F7" s="22" t="str">
-        <f t="shared" ref="F7:F71" si="4">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <f t="shared" ref="F7:F73" si="4">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
         <v/>
       </c>
       <c r="G7" s="43"/>
@@ -10990,7 +11100,7 @@
     <row r="40" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="17"/>
       <c r="B40" s="59" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C40" s="60">
         <v>1</v>
@@ -11065,7 +11175,7 @@
     <row r="41" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="17"/>
       <c r="B41" s="59" t="s">
-        <v>44</v>
+        <v>77</v>
       </c>
       <c r="C41" s="60">
         <v>1</v>
@@ -11140,7 +11250,7 @@
     <row r="42" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="17"/>
       <c r="B42" s="59" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="C42" s="60">
         <v>1</v>
@@ -11215,7 +11325,7 @@
     <row r="43" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="17"/>
       <c r="B43" s="59" t="s">
-        <v>47</v>
+        <v>79</v>
       </c>
       <c r="C43" s="60">
         <v>1</v>
@@ -11290,7 +11400,7 @@
     <row r="44" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="17"/>
       <c r="B44" s="59" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="C44" s="60">
         <v>1</v>
@@ -11740,7 +11850,7 @@
     <row r="50" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="17"/>
       <c r="B50" s="59" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C50" s="60">
         <v>1</v>
@@ -11815,16 +11925,16 @@
     <row r="51" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="17"/>
       <c r="B51" s="59" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C51" s="60">
         <v>1</v>
       </c>
       <c r="D51" s="61">
-        <v>44896</v>
+        <v>44897</v>
       </c>
       <c r="E51" s="61">
-        <v>44897</v>
+        <v>44898</v>
       </c>
       <c r="F51" s="62">
         <f t="shared" si="4"/>
@@ -11890,16 +12000,16 @@
     <row r="52" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="17"/>
       <c r="B52" s="59" t="s">
-        <v>43</v>
+        <v>82</v>
       </c>
       <c r="C52" s="60">
         <v>1</v>
       </c>
       <c r="D52" s="61">
-        <v>44896</v>
+        <v>44897</v>
       </c>
       <c r="E52" s="61">
-        <v>44897</v>
+        <v>44898</v>
       </c>
       <c r="F52" s="62">
         <f t="shared" si="4"/>
@@ -11971,10 +12081,10 @@
         <v>1</v>
       </c>
       <c r="D53" s="61">
-        <v>44896</v>
+        <v>44897</v>
       </c>
       <c r="E53" s="61">
-        <v>44897</v>
+        <v>44898</v>
       </c>
       <c r="F53" s="62">
         <f t="shared" si="4"/>
@@ -12037,21 +12147,19 @@
       <c r="BI53" s="43"/>
       <c r="BJ53" s="43"/>
     </row>
-    <row r="54" spans="1:62" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="17"/>
-      <c r="B54" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="C54" s="36"/>
-      <c r="D54" s="91">
-        <v>44899</v>
-      </c>
-      <c r="E54" s="91">
-        <v>44900</v>
-      </c>
-      <c r="F54" s="63">
+      <c r="B54" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="C54" s="60">
+        <v>0</v>
+      </c>
+      <c r="D54" s="61"/>
+      <c r="E54" s="61"/>
+      <c r="F54" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="G54" s="43"/>
       <c r="H54" s="43"/>
@@ -12112,21 +12220,17 @@
     </row>
     <row r="55" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="17"/>
-      <c r="B55" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C55" s="38">
-        <v>1</v>
-      </c>
-      <c r="D55" s="61">
-        <v>44899</v>
-      </c>
-      <c r="E55" s="61">
-        <v>44900</v>
-      </c>
-      <c r="F55" s="55">
+      <c r="B55" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="C55" s="60">
+        <v>0</v>
+      </c>
+      <c r="D55" s="61"/>
+      <c r="E55" s="61"/>
+      <c r="F55" s="62" t="str">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v/>
       </c>
       <c r="G55" s="43"/>
       <c r="H55" s="43"/>
@@ -12185,21 +12289,19 @@
       <c r="BI55" s="43"/>
       <c r="BJ55" s="43"/>
     </row>
-    <row r="56" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:62" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="17"/>
-      <c r="B56" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="C56" s="38">
-        <v>1</v>
-      </c>
-      <c r="D56" s="61">
+      <c r="B56" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C56" s="36"/>
+      <c r="D56" s="85">
         <v>44899</v>
       </c>
-      <c r="E56" s="61">
+      <c r="E56" s="85">
         <v>44900</v>
       </c>
-      <c r="F56" s="55">
+      <c r="F56" s="63">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
@@ -12263,7 +12365,7 @@
     <row r="57" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="17"/>
       <c r="B57" s="37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C57" s="38">
         <v>1</v>
@@ -12338,7 +12440,7 @@
     <row r="58" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="17"/>
       <c r="B58" s="37" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C58" s="38">
         <v>1</v>
@@ -12413,7 +12515,7 @@
     <row r="59" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="17"/>
       <c r="B59" s="37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C59" s="38">
         <v>1</v>
@@ -12485,21 +12587,23 @@
       <c r="BI59" s="43"/>
       <c r="BJ59" s="43"/>
     </row>
-    <row r="60" spans="1:62" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="17"/>
-      <c r="B60" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="C60" s="40"/>
-      <c r="D60" s="75">
-        <v>44851</v>
-      </c>
-      <c r="E60" s="75">
+      <c r="B60" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C60" s="38">
+        <v>1</v>
+      </c>
+      <c r="D60" s="61">
+        <v>44899</v>
+      </c>
+      <c r="E60" s="61">
         <v>44900</v>
       </c>
-      <c r="F60" s="76">
+      <c r="F60" s="55">
         <f t="shared" si="4"/>
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="G60" s="43"/>
       <c r="H60" s="43"/>
@@ -12560,21 +12664,21 @@
     </row>
     <row r="61" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="17"/>
-      <c r="B61" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="C61" s="42">
-        <v>1</v>
-      </c>
-      <c r="D61" s="53">
-        <v>44851</v>
-      </c>
-      <c r="E61" s="53">
+      <c r="B61" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C61" s="38">
+        <v>1</v>
+      </c>
+      <c r="D61" s="61">
+        <v>44899</v>
+      </c>
+      <c r="E61" s="61">
         <v>44900</v>
       </c>
-      <c r="F61" s="54">
+      <c r="F61" s="55">
         <f t="shared" si="4"/>
-        <v>50</v>
+        <v>2</v>
       </c>
       <c r="G61" s="43"/>
       <c r="H61" s="43"/>
@@ -12592,7 +12696,7 @@
       <c r="T61" s="43"/>
       <c r="U61" s="43"/>
       <c r="V61" s="43"/>
-      <c r="W61" s="44"/>
+      <c r="W61" s="43"/>
       <c r="X61" s="43"/>
       <c r="Y61" s="43"/>
       <c r="Z61" s="43"/>
@@ -12633,23 +12737,21 @@
       <c r="BI61" s="43"/>
       <c r="BJ61" s="43"/>
     </row>
-    <row r="62" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:62" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="17"/>
-      <c r="B62" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="C62" s="42">
-        <v>1</v>
-      </c>
-      <c r="D62" s="53">
+      <c r="B62" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C62" s="40"/>
+      <c r="D62" s="75">
         <v>44851</v>
       </c>
-      <c r="E62" s="53">
-        <v>44852</v>
-      </c>
-      <c r="F62" s="54">
+      <c r="E62" s="75">
+        <v>44900</v>
+      </c>
+      <c r="F62" s="76">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="G62" s="43"/>
       <c r="H62" s="43"/>
@@ -12711,20 +12813,20 @@
     <row r="63" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="17"/>
       <c r="B63" s="41" t="s">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="C63" s="42">
         <v>1</v>
       </c>
       <c r="D63" s="53">
-        <v>44852</v>
+        <v>44851</v>
       </c>
       <c r="E63" s="53">
-        <v>44853</v>
+        <v>44900</v>
       </c>
       <c r="F63" s="54">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="G63" s="43"/>
       <c r="H63" s="43"/>
@@ -12742,7 +12844,7 @@
       <c r="T63" s="43"/>
       <c r="U63" s="43"/>
       <c r="V63" s="43"/>
-      <c r="W63" s="43"/>
+      <c r="W63" s="44"/>
       <c r="X63" s="43"/>
       <c r="Y63" s="43"/>
       <c r="Z63" s="43"/>
@@ -12786,16 +12888,16 @@
     <row r="64" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="17"/>
       <c r="B64" s="41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C64" s="42">
         <v>1</v>
       </c>
       <c r="D64" s="53">
-        <v>44854</v>
+        <v>44851</v>
       </c>
       <c r="E64" s="53">
-        <v>44855</v>
+        <v>44852</v>
       </c>
       <c r="F64" s="54">
         <f t="shared" si="4"/>
@@ -12861,16 +12963,16 @@
     <row r="65" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="17"/>
       <c r="B65" s="41" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C65" s="42">
         <v>1</v>
       </c>
       <c r="D65" s="53">
-        <v>44856</v>
+        <v>44852</v>
       </c>
       <c r="E65" s="53">
-        <v>44857</v>
+        <v>44853</v>
       </c>
       <c r="F65" s="54">
         <f t="shared" si="4"/>
@@ -12936,20 +13038,20 @@
     <row r="66" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="17"/>
       <c r="B66" s="41" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C66" s="42">
         <v>1</v>
       </c>
       <c r="D66" s="53">
-        <v>44857</v>
+        <v>44854</v>
       </c>
       <c r="E66" s="53">
-        <v>44859</v>
+        <v>44855</v>
       </c>
       <c r="F66" s="54">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G66" s="43"/>
       <c r="H66" s="43"/>
@@ -13011,20 +13113,20 @@
     <row r="67" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="17"/>
       <c r="B67" s="41" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C67" s="42">
         <v>1</v>
       </c>
       <c r="D67" s="53">
-        <v>44860</v>
+        <v>44856</v>
       </c>
       <c r="E67" s="53">
-        <v>44865</v>
+        <v>44857</v>
       </c>
       <c r="F67" s="54">
         <f t="shared" si="4"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G67" s="43"/>
       <c r="H67" s="43"/>
@@ -13086,20 +13188,20 @@
     <row r="68" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="17"/>
       <c r="B68" s="41" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C68" s="42">
         <v>1</v>
       </c>
       <c r="D68" s="53">
-        <v>44866</v>
+        <v>44857</v>
       </c>
       <c r="E68" s="53">
-        <v>44895</v>
+        <v>44859</v>
       </c>
       <c r="F68" s="54">
         <f t="shared" si="4"/>
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="G68" s="43"/>
       <c r="H68" s="43"/>
@@ -13161,20 +13263,20 @@
     <row r="69" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="17"/>
       <c r="B69" s="41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C69" s="42">
         <v>1</v>
       </c>
       <c r="D69" s="53">
-        <v>44895</v>
+        <v>44860</v>
       </c>
       <c r="E69" s="53">
-        <v>44897</v>
+        <v>44865</v>
       </c>
       <c r="F69" s="54">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G69" s="43"/>
       <c r="H69" s="43"/>
@@ -13236,20 +13338,20 @@
     <row r="70" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="17"/>
       <c r="B70" s="41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C70" s="42">
         <v>1</v>
       </c>
       <c r="D70" s="53">
-        <v>44898</v>
+        <v>44866</v>
       </c>
       <c r="E70" s="53">
-        <v>44898</v>
+        <v>44895</v>
       </c>
       <c r="F70" s="54">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="G70" s="43"/>
       <c r="H70" s="43"/>
@@ -13311,114 +13413,264 @@
     <row r="71" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="17"/>
       <c r="B71" s="41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C71" s="42">
         <v>1</v>
       </c>
       <c r="D71" s="53">
-        <v>44899</v>
+        <v>44895</v>
       </c>
       <c r="E71" s="53">
-        <v>44900</v>
+        <v>44897</v>
       </c>
       <c r="F71" s="54">
         <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="G71" s="43"/>
+      <c r="H71" s="43"/>
+      <c r="I71" s="43"/>
+      <c r="J71" s="43"/>
+      <c r="K71" s="43"/>
+      <c r="L71" s="43"/>
+      <c r="M71" s="43"/>
+      <c r="N71" s="43"/>
+      <c r="O71" s="43"/>
+      <c r="P71" s="43"/>
+      <c r="Q71" s="43"/>
+      <c r="R71" s="43"/>
+      <c r="S71" s="43"/>
+      <c r="T71" s="43"/>
+      <c r="U71" s="43"/>
+      <c r="V71" s="43"/>
+      <c r="W71" s="43"/>
+      <c r="X71" s="43"/>
+      <c r="Y71" s="43"/>
+      <c r="Z71" s="43"/>
+      <c r="AA71" s="43"/>
+      <c r="AB71" s="43"/>
+      <c r="AC71" s="43"/>
+      <c r="AD71" s="43"/>
+      <c r="AE71" s="43"/>
+      <c r="AF71" s="43"/>
+      <c r="AG71" s="43"/>
+      <c r="AH71" s="43"/>
+      <c r="AI71" s="43"/>
+      <c r="AJ71" s="43"/>
+      <c r="AK71" s="43"/>
+      <c r="AL71" s="43"/>
+      <c r="AM71" s="43"/>
+      <c r="AN71" s="43"/>
+      <c r="AO71" s="43"/>
+      <c r="AP71" s="43"/>
+      <c r="AQ71" s="43"/>
+      <c r="AR71" s="43"/>
+      <c r="AS71" s="43"/>
+      <c r="AT71" s="43"/>
+      <c r="AU71" s="43"/>
+      <c r="AV71" s="43"/>
+      <c r="AW71" s="43"/>
+      <c r="AX71" s="43"/>
+      <c r="AY71" s="43"/>
+      <c r="AZ71" s="43"/>
+      <c r="BA71" s="43"/>
+      <c r="BB71" s="43"/>
+      <c r="BC71" s="43"/>
+      <c r="BD71" s="43"/>
+      <c r="BE71" s="43"/>
+      <c r="BF71" s="43"/>
+      <c r="BG71" s="43"/>
+      <c r="BH71" s="43"/>
+      <c r="BI71" s="43"/>
+      <c r="BJ71" s="43"/>
+    </row>
+    <row r="72" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="17"/>
+      <c r="B72" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C72" s="42">
+        <v>1</v>
+      </c>
+      <c r="D72" s="53">
+        <v>44898</v>
+      </c>
+      <c r="E72" s="53">
+        <v>44898</v>
+      </c>
+      <c r="F72" s="54">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G72" s="43"/>
+      <c r="H72" s="43"/>
+      <c r="I72" s="43"/>
+      <c r="J72" s="43"/>
+      <c r="K72" s="43"/>
+      <c r="L72" s="43"/>
+      <c r="M72" s="43"/>
+      <c r="N72" s="43"/>
+      <c r="O72" s="43"/>
+      <c r="P72" s="43"/>
+      <c r="Q72" s="43"/>
+      <c r="R72" s="43"/>
+      <c r="S72" s="43"/>
+      <c r="T72" s="43"/>
+      <c r="U72" s="43"/>
+      <c r="V72" s="43"/>
+      <c r="W72" s="43"/>
+      <c r="X72" s="43"/>
+      <c r="Y72" s="43"/>
+      <c r="Z72" s="43"/>
+      <c r="AA72" s="43"/>
+      <c r="AB72" s="43"/>
+      <c r="AC72" s="43"/>
+      <c r="AD72" s="43"/>
+      <c r="AE72" s="43"/>
+      <c r="AF72" s="43"/>
+      <c r="AG72" s="43"/>
+      <c r="AH72" s="43"/>
+      <c r="AI72" s="43"/>
+      <c r="AJ72" s="43"/>
+      <c r="AK72" s="43"/>
+      <c r="AL72" s="43"/>
+      <c r="AM72" s="43"/>
+      <c r="AN72" s="43"/>
+      <c r="AO72" s="43"/>
+      <c r="AP72" s="43"/>
+      <c r="AQ72" s="43"/>
+      <c r="AR72" s="43"/>
+      <c r="AS72" s="43"/>
+      <c r="AT72" s="43"/>
+      <c r="AU72" s="43"/>
+      <c r="AV72" s="43"/>
+      <c r="AW72" s="43"/>
+      <c r="AX72" s="43"/>
+      <c r="AY72" s="43"/>
+      <c r="AZ72" s="43"/>
+      <c r="BA72" s="43"/>
+      <c r="BB72" s="43"/>
+      <c r="BC72" s="43"/>
+      <c r="BD72" s="43"/>
+      <c r="BE72" s="43"/>
+      <c r="BF72" s="43"/>
+      <c r="BG72" s="43"/>
+      <c r="BH72" s="43"/>
+      <c r="BI72" s="43"/>
+      <c r="BJ72" s="43"/>
+    </row>
+    <row r="73" spans="1:62" s="2" customFormat="1" ht="21.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="17"/>
+      <c r="B73" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C73" s="42">
+        <v>1</v>
+      </c>
+      <c r="D73" s="53">
+        <v>44899</v>
+      </c>
+      <c r="E73" s="53">
+        <v>44900</v>
+      </c>
+      <c r="F73" s="54">
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="G71" s="45"/>
-      <c r="H71" s="45"/>
-      <c r="I71" s="45"/>
-      <c r="J71" s="45"/>
-      <c r="K71" s="45"/>
-      <c r="L71" s="45"/>
-      <c r="M71" s="45"/>
-      <c r="N71" s="45"/>
-      <c r="O71" s="45"/>
-      <c r="P71" s="45"/>
-      <c r="Q71" s="45"/>
-      <c r="R71" s="45"/>
-      <c r="S71" s="45"/>
-      <c r="T71" s="45"/>
-      <c r="U71" s="45"/>
-      <c r="V71" s="45"/>
-      <c r="W71" s="45"/>
-      <c r="X71" s="45"/>
-      <c r="Y71" s="45"/>
-      <c r="Z71" s="45"/>
-      <c r="AA71" s="45"/>
-      <c r="AB71" s="45"/>
-      <c r="AC71" s="45"/>
-      <c r="AD71" s="45"/>
-      <c r="AE71" s="45"/>
-      <c r="AF71" s="45"/>
-      <c r="AG71" s="45"/>
-      <c r="AH71" s="45"/>
-      <c r="AI71" s="45"/>
-      <c r="AJ71" s="45"/>
-      <c r="AK71" s="45"/>
-      <c r="AL71" s="45"/>
-      <c r="AM71" s="45"/>
-      <c r="AN71" s="45"/>
-      <c r="AO71" s="45"/>
-      <c r="AP71" s="45"/>
-      <c r="AQ71" s="45"/>
-      <c r="AR71" s="45"/>
-      <c r="AS71" s="45"/>
-      <c r="AT71" s="45"/>
-      <c r="AU71" s="45"/>
-      <c r="AV71" s="45"/>
-      <c r="AW71" s="45"/>
-      <c r="AX71" s="45"/>
-      <c r="AY71" s="45"/>
-      <c r="AZ71" s="45"/>
-      <c r="BA71" s="45"/>
-      <c r="BB71" s="45"/>
-      <c r="BC71" s="45"/>
-      <c r="BD71" s="45"/>
-      <c r="BE71" s="45"/>
-      <c r="BF71" s="45"/>
-      <c r="BG71" s="45"/>
-      <c r="BH71" s="45"/>
-      <c r="BI71" s="45"/>
-      <c r="BJ71" s="45"/>
-    </row>
-    <row r="72" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-    </row>
-    <row r="73" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="B73" s="16" t="s">
+      <c r="G73" s="45"/>
+      <c r="H73" s="45"/>
+      <c r="I73" s="45"/>
+      <c r="J73" s="45"/>
+      <c r="K73" s="45"/>
+      <c r="L73" s="45"/>
+      <c r="M73" s="45"/>
+      <c r="N73" s="45"/>
+      <c r="O73" s="45"/>
+      <c r="P73" s="45"/>
+      <c r="Q73" s="45"/>
+      <c r="R73" s="45"/>
+      <c r="S73" s="45"/>
+      <c r="T73" s="45"/>
+      <c r="U73" s="45"/>
+      <c r="V73" s="45"/>
+      <c r="W73" s="45"/>
+      <c r="X73" s="45"/>
+      <c r="Y73" s="45"/>
+      <c r="Z73" s="45"/>
+      <c r="AA73" s="45"/>
+      <c r="AB73" s="45"/>
+      <c r="AC73" s="45"/>
+      <c r="AD73" s="45"/>
+      <c r="AE73" s="45"/>
+      <c r="AF73" s="45"/>
+      <c r="AG73" s="45"/>
+      <c r="AH73" s="45"/>
+      <c r="AI73" s="45"/>
+      <c r="AJ73" s="45"/>
+      <c r="AK73" s="45"/>
+      <c r="AL73" s="45"/>
+      <c r="AM73" s="45"/>
+      <c r="AN73" s="45"/>
+      <c r="AO73" s="45"/>
+      <c r="AP73" s="45"/>
+      <c r="AQ73" s="45"/>
+      <c r="AR73" s="45"/>
+      <c r="AS73" s="45"/>
+      <c r="AT73" s="45"/>
+      <c r="AU73" s="45"/>
+      <c r="AV73" s="45"/>
+      <c r="AW73" s="45"/>
+      <c r="AX73" s="45"/>
+      <c r="AY73" s="45"/>
+      <c r="AZ73" s="45"/>
+      <c r="BA73" s="45"/>
+      <c r="BB73" s="45"/>
+      <c r="BC73" s="45"/>
+      <c r="BD73" s="45"/>
+      <c r="BE73" s="45"/>
+      <c r="BF73" s="45"/>
+      <c r="BG73" s="45"/>
+      <c r="BH73" s="45"/>
+      <c r="BI73" s="45"/>
+      <c r="BJ73" s="45"/>
+    </row>
+    <row r="74" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A74" s="5"/>
+    </row>
+    <row r="75" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="B75" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E73" s="47">
+      <c r="E75" s="47">
         <v>43113</v>
       </c>
     </row>
-    <row r="74" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="B74" s="50" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:62" x14ac:dyDescent="0.25">
-      <c r="B75" s="49" t="s">
+    <row r="76" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="B76" s="50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="B77" s="49" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AB4:AH4"/>
+    <mergeCell ref="AI4:AO4"/>
+    <mergeCell ref="AP4:AV4"/>
+    <mergeCell ref="AW4:BC4"/>
+    <mergeCell ref="BD4:BJ4"/>
     <mergeCell ref="H1:Y1"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="G4:M4"/>
     <mergeCell ref="N4:T4"/>
     <mergeCell ref="U4:AA4"/>
-    <mergeCell ref="AB4:AH4"/>
-    <mergeCell ref="AI4:AO4"/>
-    <mergeCell ref="AP4:AV4"/>
-    <mergeCell ref="AW4:BC4"/>
-    <mergeCell ref="BD4:BJ4"/>
   </mergeCells>
-  <conditionalFormatting sqref="C7:C18 C20:C24 C26:C31 C38 C41:C44 C46:C49 C52:C71 C33:C36">
+  <conditionalFormatting sqref="C7:C18 C20:C24 C26:C31 C38 C41:C44 C46:C49 C33:C36 C52:C73">
     <cfRule type="dataBar" priority="31">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -13432,16 +13684,16 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7:BJ31 G38:BJ38 G41:BJ44 G46:BJ49 G52:BJ71 G33:BJ36">
-    <cfRule type="expression" dxfId="23" priority="32">
+  <conditionalFormatting sqref="G7:BJ31 G38:BJ38 G41:BJ44 G46:BJ49 G52:BJ73 G33:BJ36">
+    <cfRule type="expression" dxfId="26" priority="32">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="33" stopIfTrue="1">
       <formula>AND(task_end&gt;=G$5,task_start&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5:BJ31 G38:BJ38 G41:BJ44 G46:BJ49 G52:BJ71 G33:BJ36">
-    <cfRule type="expression" dxfId="21" priority="34">
+  <conditionalFormatting sqref="G5:BJ31 G38:BJ38 G41:BJ44 G46:BJ49 G52:BJ73 G33:BJ36">
+    <cfRule type="expression" dxfId="24" priority="34">
       <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13502,28 +13754,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:BJ32">
-    <cfRule type="expression" dxfId="20" priority="26">
+    <cfRule type="expression" dxfId="23" priority="26">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="27" stopIfTrue="1">
       <formula>AND(task_end&gt;=G$5,task_start&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G32:BJ32">
-    <cfRule type="expression" dxfId="18" priority="28">
+    <cfRule type="expression" dxfId="21" priority="28">
       <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39:BJ39">
-    <cfRule type="expression" dxfId="17" priority="22">
+    <cfRule type="expression" dxfId="20" priority="22">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="23" stopIfTrue="1">
       <formula>AND(task_end&gt;=G$5,task_start&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39:BJ39">
-    <cfRule type="expression" dxfId="15" priority="24">
+    <cfRule type="expression" dxfId="18" priority="24">
       <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13542,15 +13794,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37:BJ37">
-    <cfRule type="expression" dxfId="14" priority="18">
+    <cfRule type="expression" dxfId="17" priority="18">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="19" stopIfTrue="1">
       <formula>AND(task_end&gt;=G$5,task_start&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37:BJ37">
-    <cfRule type="expression" dxfId="12" priority="20">
+    <cfRule type="expression" dxfId="15" priority="20">
       <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13569,15 +13821,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40:BJ40">
-    <cfRule type="expression" dxfId="11" priority="14">
+    <cfRule type="expression" dxfId="14" priority="14">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="15" stopIfTrue="1">
       <formula>AND(task_end&gt;=G$5,task_start&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40:BJ40">
-    <cfRule type="expression" dxfId="9" priority="16">
+    <cfRule type="expression" dxfId="12" priority="16">
       <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13596,15 +13848,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45:BJ45">
-    <cfRule type="expression" dxfId="8" priority="10">
+    <cfRule type="expression" dxfId="11" priority="10">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="11" stopIfTrue="1">
       <formula>AND(task_end&gt;=G$5,task_start&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G45:BJ45">
-    <cfRule type="expression" dxfId="6" priority="12">
+    <cfRule type="expression" dxfId="9" priority="12">
       <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13623,15 +13875,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50:BJ50">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="8" priority="6">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="7" stopIfTrue="1">
       <formula>AND(task_end&gt;=G$5,task_start&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G50:BJ50">
-    <cfRule type="expression" dxfId="3" priority="8">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13650,15 +13902,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51:BJ51">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
       <formula>AND(task_end&gt;=G$5,task_start&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G51:BJ51">
-    <cfRule type="expression" dxfId="0" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13668,8 +13920,8 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B74" r:id="rId1" xr:uid="{B59DE972-1BED-491D-8C00-5C2D97AE7CB5}"/>
-    <hyperlink ref="B73" r:id="rId2" xr:uid="{6D48BA4D-4454-4BF5-9A24-E758F374CA69}"/>
+    <hyperlink ref="B76" r:id="rId1" xr:uid="{B59DE972-1BED-491D-8C00-5C2D97AE7CB5}"/>
+    <hyperlink ref="B75" r:id="rId2" xr:uid="{6D48BA4D-4454-4BF5-9A24-E758F374CA69}"/>
   </hyperlinks>
   <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="58" fitToHeight="0" orientation="landscape" r:id="rId3"/>
@@ -13691,7 +13943,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C7:C18 C20:C24 C26:C31 C38 C41:C44 C46:C49 C52:C71 C33:C36</xm:sqref>
+          <xm:sqref>C7:C18 C20:C24 C26:C31 C38 C41:C44 C46:C49 C33:C36 C52:C73</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{4851E6B4-6440-46A0-B6C9-F3BECC355CD6}">
@@ -13832,4 +14084,1623 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F4A3915-93AC-407B-9B03-B1A884C80028}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:BJ22"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AQ18" sqref="B1:AV18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.140625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" customWidth="1"/>
+    <col min="7" max="62" width="2.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:62" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="46"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="86"/>
+      <c r="O1" s="86"/>
+      <c r="P1" s="86"/>
+      <c r="Q1" s="86"/>
+      <c r="R1" s="86"/>
+      <c r="S1" s="86"/>
+      <c r="T1" s="86"/>
+      <c r="U1" s="86"/>
+      <c r="V1" s="86"/>
+      <c r="W1" s="86"/>
+      <c r="X1" s="86"/>
+      <c r="Y1" s="86"/>
+    </row>
+    <row r="2" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="90">
+        <v>44935</v>
+      </c>
+      <c r="E2" s="91"/>
+    </row>
+    <row r="3" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="90">
+        <v>44969</v>
+      </c>
+      <c r="E3" s="91"/>
+    </row>
+    <row r="4" spans="1:62" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="87">
+        <f>G5</f>
+        <v>44935</v>
+      </c>
+      <c r="H4" s="88"/>
+      <c r="I4" s="88"/>
+      <c r="J4" s="88"/>
+      <c r="K4" s="88"/>
+      <c r="L4" s="88"/>
+      <c r="M4" s="89"/>
+      <c r="N4" s="87">
+        <f>N5</f>
+        <v>44942</v>
+      </c>
+      <c r="O4" s="88"/>
+      <c r="P4" s="88"/>
+      <c r="Q4" s="88"/>
+      <c r="R4" s="88"/>
+      <c r="S4" s="88"/>
+      <c r="T4" s="89"/>
+      <c r="U4" s="87">
+        <f>U5</f>
+        <v>44949</v>
+      </c>
+      <c r="V4" s="88"/>
+      <c r="W4" s="88"/>
+      <c r="X4" s="88"/>
+      <c r="Y4" s="88"/>
+      <c r="Z4" s="88"/>
+      <c r="AA4" s="89"/>
+      <c r="AB4" s="87">
+        <f>AB5</f>
+        <v>44956</v>
+      </c>
+      <c r="AC4" s="88"/>
+      <c r="AD4" s="88"/>
+      <c r="AE4" s="88"/>
+      <c r="AF4" s="88"/>
+      <c r="AG4" s="88"/>
+      <c r="AH4" s="89"/>
+      <c r="AI4" s="87">
+        <f>AI5</f>
+        <v>44963</v>
+      </c>
+      <c r="AJ4" s="88"/>
+      <c r="AK4" s="88"/>
+      <c r="AL4" s="88"/>
+      <c r="AM4" s="88"/>
+      <c r="AN4" s="88"/>
+      <c r="AO4" s="89"/>
+      <c r="AP4" s="87">
+        <f>AP5</f>
+        <v>44970</v>
+      </c>
+      <c r="AQ4" s="88"/>
+      <c r="AR4" s="88"/>
+      <c r="AS4" s="88"/>
+      <c r="AT4" s="88"/>
+      <c r="AU4" s="88"/>
+      <c r="AV4" s="89"/>
+      <c r="AW4" s="87">
+        <f>AW5</f>
+        <v>44977</v>
+      </c>
+      <c r="AX4" s="88"/>
+      <c r="AY4" s="88"/>
+      <c r="AZ4" s="88"/>
+      <c r="BA4" s="88"/>
+      <c r="BB4" s="88"/>
+      <c r="BC4" s="89"/>
+      <c r="BD4" s="87">
+        <f>BD5</f>
+        <v>44984</v>
+      </c>
+      <c r="BE4" s="88"/>
+      <c r="BF4" s="88"/>
+      <c r="BG4" s="88"/>
+      <c r="BH4" s="88"/>
+      <c r="BI4" s="88"/>
+      <c r="BJ4" s="89"/>
+    </row>
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="G5" s="12">
+        <f>D2-WEEKDAY(D2,1)+2+7*(D4-1)</f>
+        <v>44935</v>
+      </c>
+      <c r="H5" s="11">
+        <f>G5+1</f>
+        <v>44936</v>
+      </c>
+      <c r="I5" s="11">
+        <f t="shared" ref="I5:AV5" si="0">H5+1</f>
+        <v>44937</v>
+      </c>
+      <c r="J5" s="11">
+        <f t="shared" si="0"/>
+        <v>44938</v>
+      </c>
+      <c r="K5" s="11">
+        <f t="shared" si="0"/>
+        <v>44939</v>
+      </c>
+      <c r="L5" s="11">
+        <f t="shared" si="0"/>
+        <v>44940</v>
+      </c>
+      <c r="M5" s="13">
+        <f t="shared" si="0"/>
+        <v>44941</v>
+      </c>
+      <c r="N5" s="12">
+        <f>M5+1</f>
+        <v>44942</v>
+      </c>
+      <c r="O5" s="11">
+        <f>N5+1</f>
+        <v>44943</v>
+      </c>
+      <c r="P5" s="11">
+        <f t="shared" si="0"/>
+        <v>44944</v>
+      </c>
+      <c r="Q5" s="11">
+        <f t="shared" si="0"/>
+        <v>44945</v>
+      </c>
+      <c r="R5" s="11">
+        <f t="shared" si="0"/>
+        <v>44946</v>
+      </c>
+      <c r="S5" s="11">
+        <f t="shared" si="0"/>
+        <v>44947</v>
+      </c>
+      <c r="T5" s="13">
+        <f t="shared" si="0"/>
+        <v>44948</v>
+      </c>
+      <c r="U5" s="12">
+        <f>T5+1</f>
+        <v>44949</v>
+      </c>
+      <c r="V5" s="11">
+        <f>U5+1</f>
+        <v>44950</v>
+      </c>
+      <c r="W5" s="11">
+        <f t="shared" si="0"/>
+        <v>44951</v>
+      </c>
+      <c r="X5" s="11">
+        <f t="shared" si="0"/>
+        <v>44952</v>
+      </c>
+      <c r="Y5" s="11">
+        <f t="shared" si="0"/>
+        <v>44953</v>
+      </c>
+      <c r="Z5" s="11">
+        <f t="shared" si="0"/>
+        <v>44954</v>
+      </c>
+      <c r="AA5" s="13">
+        <f t="shared" si="0"/>
+        <v>44955</v>
+      </c>
+      <c r="AB5" s="12">
+        <f>AA5+1</f>
+        <v>44956</v>
+      </c>
+      <c r="AC5" s="11">
+        <f>AB5+1</f>
+        <v>44957</v>
+      </c>
+      <c r="AD5" s="11">
+        <f t="shared" si="0"/>
+        <v>44958</v>
+      </c>
+      <c r="AE5" s="11">
+        <f t="shared" si="0"/>
+        <v>44959</v>
+      </c>
+      <c r="AF5" s="11">
+        <f t="shared" si="0"/>
+        <v>44960</v>
+      </c>
+      <c r="AG5" s="11">
+        <f t="shared" si="0"/>
+        <v>44961</v>
+      </c>
+      <c r="AH5" s="13">
+        <f t="shared" si="0"/>
+        <v>44962</v>
+      </c>
+      <c r="AI5" s="12">
+        <f>AH5+1</f>
+        <v>44963</v>
+      </c>
+      <c r="AJ5" s="11">
+        <f>AI5+1</f>
+        <v>44964</v>
+      </c>
+      <c r="AK5" s="11">
+        <f t="shared" si="0"/>
+        <v>44965</v>
+      </c>
+      <c r="AL5" s="11">
+        <f t="shared" si="0"/>
+        <v>44966</v>
+      </c>
+      <c r="AM5" s="11">
+        <f t="shared" si="0"/>
+        <v>44967</v>
+      </c>
+      <c r="AN5" s="11">
+        <f t="shared" si="0"/>
+        <v>44968</v>
+      </c>
+      <c r="AO5" s="13">
+        <f t="shared" si="0"/>
+        <v>44969</v>
+      </c>
+      <c r="AP5" s="12">
+        <f>AO5+1</f>
+        <v>44970</v>
+      </c>
+      <c r="AQ5" s="11">
+        <f>AP5+1</f>
+        <v>44971</v>
+      </c>
+      <c r="AR5" s="11">
+        <f t="shared" si="0"/>
+        <v>44972</v>
+      </c>
+      <c r="AS5" s="11">
+        <f t="shared" si="0"/>
+        <v>44973</v>
+      </c>
+      <c r="AT5" s="11">
+        <f t="shared" si="0"/>
+        <v>44974</v>
+      </c>
+      <c r="AU5" s="11">
+        <f t="shared" si="0"/>
+        <v>44975</v>
+      </c>
+      <c r="AV5" s="13">
+        <f t="shared" si="0"/>
+        <v>44976</v>
+      </c>
+      <c r="AW5" s="12">
+        <f>AV5+1</f>
+        <v>44977</v>
+      </c>
+      <c r="AX5" s="11">
+        <f>AW5+1</f>
+        <v>44978</v>
+      </c>
+      <c r="AY5" s="11">
+        <f t="shared" ref="AY5:BC5" si="1">AX5+1</f>
+        <v>44979</v>
+      </c>
+      <c r="AZ5" s="11">
+        <f t="shared" si="1"/>
+        <v>44980</v>
+      </c>
+      <c r="BA5" s="11">
+        <f t="shared" si="1"/>
+        <v>44981</v>
+      </c>
+      <c r="BB5" s="11">
+        <f t="shared" si="1"/>
+        <v>44982</v>
+      </c>
+      <c r="BC5" s="13">
+        <f t="shared" si="1"/>
+        <v>44983</v>
+      </c>
+      <c r="BD5" s="12">
+        <f>BC5+1</f>
+        <v>44984</v>
+      </c>
+      <c r="BE5" s="11">
+        <f>BD5+1</f>
+        <v>44985</v>
+      </c>
+      <c r="BF5" s="11">
+        <f t="shared" ref="BF5:BJ5" si="2">BE5+1</f>
+        <v>44986</v>
+      </c>
+      <c r="BG5" s="11">
+        <f t="shared" si="2"/>
+        <v>44987</v>
+      </c>
+      <c r="BH5" s="11">
+        <f t="shared" si="2"/>
+        <v>44988</v>
+      </c>
+      <c r="BI5" s="11">
+        <f t="shared" si="2"/>
+        <v>44989</v>
+      </c>
+      <c r="BJ5" s="13">
+        <f t="shared" si="2"/>
+        <v>44990</v>
+      </c>
+    </row>
+    <row r="6" spans="1:62" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17"/>
+      <c r="B6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="14" t="str">
+        <f t="shared" ref="G6:BJ6" si="3">LEFT(TEXT(G5,"ddd"),1)</f>
+        <v>l</v>
+      </c>
+      <c r="H6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>m</v>
+      </c>
+      <c r="I6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>m</v>
+      </c>
+      <c r="J6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>j</v>
+      </c>
+      <c r="K6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>v</v>
+      </c>
+      <c r="L6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>s</v>
+      </c>
+      <c r="M6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>d</v>
+      </c>
+      <c r="N6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>l</v>
+      </c>
+      <c r="O6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>m</v>
+      </c>
+      <c r="P6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>m</v>
+      </c>
+      <c r="Q6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>j</v>
+      </c>
+      <c r="R6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>v</v>
+      </c>
+      <c r="S6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>s</v>
+      </c>
+      <c r="T6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>d</v>
+      </c>
+      <c r="U6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>l</v>
+      </c>
+      <c r="V6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>m</v>
+      </c>
+      <c r="W6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>m</v>
+      </c>
+      <c r="X6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>j</v>
+      </c>
+      <c r="Y6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>v</v>
+      </c>
+      <c r="Z6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>s</v>
+      </c>
+      <c r="AA6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>d</v>
+      </c>
+      <c r="AB6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>l</v>
+      </c>
+      <c r="AC6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>m</v>
+      </c>
+      <c r="AD6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>m</v>
+      </c>
+      <c r="AE6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>j</v>
+      </c>
+      <c r="AF6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>v</v>
+      </c>
+      <c r="AG6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>s</v>
+      </c>
+      <c r="AH6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>d</v>
+      </c>
+      <c r="AI6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>l</v>
+      </c>
+      <c r="AJ6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>m</v>
+      </c>
+      <c r="AK6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>m</v>
+      </c>
+      <c r="AL6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>j</v>
+      </c>
+      <c r="AM6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>v</v>
+      </c>
+      <c r="AN6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>s</v>
+      </c>
+      <c r="AO6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>d</v>
+      </c>
+      <c r="AP6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>l</v>
+      </c>
+      <c r="AQ6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>m</v>
+      </c>
+      <c r="AR6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>m</v>
+      </c>
+      <c r="AS6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>j</v>
+      </c>
+      <c r="AT6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>v</v>
+      </c>
+      <c r="AU6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>s</v>
+      </c>
+      <c r="AV6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>d</v>
+      </c>
+      <c r="AW6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>l</v>
+      </c>
+      <c r="AX6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>m</v>
+      </c>
+      <c r="AY6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>m</v>
+      </c>
+      <c r="AZ6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>j</v>
+      </c>
+      <c r="BA6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>v</v>
+      </c>
+      <c r="BB6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>s</v>
+      </c>
+      <c r="BC6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>d</v>
+      </c>
+      <c r="BD6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>l</v>
+      </c>
+      <c r="BE6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>m</v>
+      </c>
+      <c r="BF6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>m</v>
+      </c>
+      <c r="BG6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>j</v>
+      </c>
+      <c r="BH6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>v</v>
+      </c>
+      <c r="BI6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>s</v>
+      </c>
+      <c r="BJ6" s="14" t="str">
+        <f t="shared" si="3"/>
+        <v>d</v>
+      </c>
+    </row>
+    <row r="7" spans="1:62" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="59" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="60">
+        <v>1</v>
+      </c>
+      <c r="D7" s="61">
+        <v>44935</v>
+      </c>
+      <c r="E7" s="61">
+        <v>44954</v>
+      </c>
+      <c r="F7" s="62">
+        <f t="shared" ref="F7:F18" si="4">IF(OR(ISBLANK(task_start),ISBLANK(task_end)),"",task_end-task_start+1)</f>
+        <v>20</v>
+      </c>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
+      <c r="K7" s="43"/>
+      <c r="L7" s="43"/>
+      <c r="M7" s="43"/>
+      <c r="N7" s="43"/>
+      <c r="O7" s="43"/>
+      <c r="P7" s="43"/>
+      <c r="Q7" s="43"/>
+      <c r="R7" s="43"/>
+      <c r="S7" s="43"/>
+      <c r="T7" s="43"/>
+      <c r="U7" s="43"/>
+      <c r="V7" s="43"/>
+      <c r="W7" s="43"/>
+      <c r="X7" s="43"/>
+      <c r="Y7" s="43"/>
+      <c r="Z7" s="43"/>
+      <c r="AA7" s="43"/>
+      <c r="AB7" s="43"/>
+      <c r="AC7" s="43"/>
+      <c r="AD7" s="43"/>
+      <c r="AE7" s="43"/>
+      <c r="AF7" s="43"/>
+      <c r="AG7" s="43"/>
+      <c r="AH7" s="43"/>
+      <c r="AI7" s="43"/>
+      <c r="AJ7" s="43"/>
+      <c r="AK7" s="43"/>
+      <c r="AL7" s="43"/>
+      <c r="AM7" s="43"/>
+      <c r="AN7" s="43"/>
+      <c r="AO7" s="43"/>
+      <c r="AP7" s="43"/>
+      <c r="AQ7" s="43"/>
+      <c r="AR7" s="43"/>
+      <c r="AS7" s="43"/>
+      <c r="AT7" s="43"/>
+      <c r="AU7" s="43"/>
+      <c r="AV7" s="43"/>
+      <c r="AW7" s="43"/>
+      <c r="AX7" s="43"/>
+      <c r="AY7" s="43"/>
+      <c r="AZ7" s="43"/>
+      <c r="BA7" s="43"/>
+      <c r="BB7" s="43"/>
+      <c r="BC7" s="43"/>
+      <c r="BD7" s="43"/>
+      <c r="BE7" s="43"/>
+      <c r="BF7" s="43"/>
+      <c r="BG7" s="43"/>
+      <c r="BH7" s="43"/>
+      <c r="BI7" s="43"/>
+      <c r="BJ7" s="43"/>
+    </row>
+    <row r="8" spans="1:62" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="59" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="60">
+        <v>0</v>
+      </c>
+      <c r="D8" s="61"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="62" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
+      <c r="M8" s="43"/>
+      <c r="N8" s="43"/>
+      <c r="O8" s="43"/>
+      <c r="P8" s="43"/>
+      <c r="Q8" s="43"/>
+      <c r="R8" s="43"/>
+      <c r="S8" s="43"/>
+      <c r="T8" s="43"/>
+      <c r="U8" s="43"/>
+      <c r="V8" s="43"/>
+      <c r="W8" s="43"/>
+      <c r="X8" s="43"/>
+      <c r="Y8" s="43"/>
+      <c r="Z8" s="43"/>
+      <c r="AA8" s="43"/>
+      <c r="AB8" s="43"/>
+      <c r="AC8" s="43"/>
+      <c r="AD8" s="43"/>
+      <c r="AE8" s="43"/>
+      <c r="AF8" s="43"/>
+      <c r="AG8" s="43"/>
+      <c r="AH8" s="43"/>
+      <c r="AI8" s="43"/>
+      <c r="AJ8" s="43"/>
+      <c r="AK8" s="43"/>
+      <c r="AL8" s="43"/>
+      <c r="AM8" s="43"/>
+      <c r="AN8" s="43"/>
+      <c r="AO8" s="43"/>
+      <c r="AP8" s="43"/>
+      <c r="AQ8" s="43"/>
+      <c r="AR8" s="43"/>
+      <c r="AS8" s="43"/>
+      <c r="AT8" s="43"/>
+      <c r="AU8" s="43"/>
+      <c r="AV8" s="43"/>
+      <c r="AW8" s="43"/>
+      <c r="AX8" s="43"/>
+      <c r="AY8" s="43"/>
+      <c r="AZ8" s="43"/>
+      <c r="BA8" s="43"/>
+      <c r="BB8" s="43"/>
+      <c r="BC8" s="43"/>
+      <c r="BD8" s="43"/>
+      <c r="BE8" s="43"/>
+      <c r="BF8" s="43"/>
+      <c r="BG8" s="43"/>
+      <c r="BH8" s="43"/>
+      <c r="BI8" s="43"/>
+      <c r="BJ8" s="43"/>
+    </row>
+    <row r="9" spans="1:62" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="59" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="60">
+        <v>0</v>
+      </c>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="62" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="G9" s="43"/>
+      <c r="H9" s="43"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="43"/>
+      <c r="K9" s="43"/>
+      <c r="L9" s="43"/>
+      <c r="M9" s="43"/>
+      <c r="N9" s="43"/>
+      <c r="O9" s="43"/>
+      <c r="P9" s="43"/>
+      <c r="Q9" s="43"/>
+      <c r="R9" s="43"/>
+      <c r="S9" s="43"/>
+      <c r="T9" s="43"/>
+      <c r="U9" s="43"/>
+      <c r="V9" s="43"/>
+      <c r="W9" s="43"/>
+      <c r="X9" s="43"/>
+      <c r="Y9" s="43"/>
+      <c r="Z9" s="43"/>
+      <c r="AA9" s="43"/>
+      <c r="AB9" s="43"/>
+      <c r="AC9" s="43"/>
+      <c r="AD9" s="43"/>
+      <c r="AE9" s="43"/>
+      <c r="AF9" s="43"/>
+      <c r="AG9" s="43"/>
+      <c r="AH9" s="43"/>
+      <c r="AI9" s="43"/>
+      <c r="AJ9" s="43"/>
+      <c r="AK9" s="43"/>
+      <c r="AL9" s="43"/>
+      <c r="AM9" s="43"/>
+      <c r="AN9" s="43"/>
+      <c r="AO9" s="43"/>
+      <c r="AP9" s="43"/>
+      <c r="AQ9" s="43"/>
+      <c r="AR9" s="43"/>
+      <c r="AS9" s="43"/>
+      <c r="AT9" s="43"/>
+      <c r="AU9" s="43"/>
+      <c r="AV9" s="43"/>
+      <c r="AW9" s="43"/>
+      <c r="AX9" s="43"/>
+      <c r="AY9" s="43"/>
+      <c r="AZ9" s="43"/>
+      <c r="BA9" s="43"/>
+      <c r="BB9" s="43"/>
+      <c r="BC9" s="43"/>
+      <c r="BD9" s="43"/>
+      <c r="BE9" s="43"/>
+      <c r="BF9" s="43"/>
+      <c r="BG9" s="43"/>
+      <c r="BH9" s="43"/>
+      <c r="BI9" s="43"/>
+      <c r="BJ9" s="43"/>
+    </row>
+    <row r="10" spans="1:62" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="36"/>
+      <c r="D10" s="85">
+        <v>44956</v>
+      </c>
+      <c r="E10" s="85">
+        <v>44957</v>
+      </c>
+      <c r="F10" s="63">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G10" s="43"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="43"/>
+      <c r="K10" s="43"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="43"/>
+      <c r="N10" s="43"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="43"/>
+      <c r="Q10" s="43"/>
+      <c r="R10" s="43"/>
+      <c r="S10" s="43"/>
+      <c r="T10" s="43"/>
+      <c r="U10" s="43"/>
+      <c r="V10" s="43"/>
+      <c r="W10" s="43"/>
+      <c r="X10" s="43"/>
+      <c r="Y10" s="43"/>
+      <c r="Z10" s="43"/>
+      <c r="AA10" s="43"/>
+      <c r="AB10" s="43"/>
+      <c r="AC10" s="43"/>
+      <c r="AD10" s="43"/>
+      <c r="AE10" s="43"/>
+      <c r="AF10" s="43"/>
+      <c r="AG10" s="43"/>
+      <c r="AH10" s="43"/>
+      <c r="AI10" s="43"/>
+      <c r="AJ10" s="43"/>
+      <c r="AK10" s="43"/>
+      <c r="AL10" s="43"/>
+      <c r="AM10" s="43"/>
+      <c r="AN10" s="43"/>
+      <c r="AO10" s="43"/>
+      <c r="AP10" s="43"/>
+      <c r="AQ10" s="43"/>
+      <c r="AR10" s="43"/>
+      <c r="AS10" s="43"/>
+      <c r="AT10" s="43"/>
+      <c r="AU10" s="43"/>
+      <c r="AV10" s="43"/>
+      <c r="AW10" s="43"/>
+      <c r="AX10" s="43"/>
+      <c r="AY10" s="43"/>
+      <c r="AZ10" s="43"/>
+      <c r="BA10" s="43"/>
+      <c r="BB10" s="43"/>
+      <c r="BC10" s="43"/>
+      <c r="BD10" s="43"/>
+      <c r="BE10" s="43"/>
+      <c r="BF10" s="43"/>
+      <c r="BG10" s="43"/>
+      <c r="BH10" s="43"/>
+      <c r="BI10" s="43"/>
+      <c r="BJ10" s="43"/>
+    </row>
+    <row r="11" spans="1:62" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="38">
+        <v>1</v>
+      </c>
+      <c r="D11" s="85">
+        <v>44956</v>
+      </c>
+      <c r="E11" s="85">
+        <v>44957</v>
+      </c>
+      <c r="F11" s="55">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="R11" s="43"/>
+      <c r="S11" s="43"/>
+      <c r="T11" s="43"/>
+      <c r="U11" s="43"/>
+      <c r="V11" s="43"/>
+      <c r="W11" s="43"/>
+      <c r="X11" s="43"/>
+      <c r="Y11" s="43"/>
+      <c r="Z11" s="43"/>
+      <c r="AA11" s="43"/>
+      <c r="AB11" s="43"/>
+      <c r="AC11" s="43"/>
+      <c r="AD11" s="43"/>
+      <c r="AE11" s="43"/>
+      <c r="AF11" s="43"/>
+      <c r="AG11" s="43"/>
+      <c r="AH11" s="43"/>
+      <c r="AI11" s="43"/>
+      <c r="AJ11" s="43"/>
+      <c r="AK11" s="43"/>
+      <c r="AL11" s="43"/>
+      <c r="AM11" s="43"/>
+      <c r="AN11" s="43"/>
+      <c r="AO11" s="43"/>
+      <c r="AP11" s="43"/>
+      <c r="AQ11" s="43"/>
+      <c r="AR11" s="43"/>
+      <c r="AS11" s="43"/>
+      <c r="AT11" s="43"/>
+      <c r="AU11" s="43"/>
+      <c r="AV11" s="43"/>
+      <c r="AW11" s="43"/>
+      <c r="AX11" s="43"/>
+      <c r="AY11" s="43"/>
+      <c r="AZ11" s="43"/>
+      <c r="BA11" s="43"/>
+      <c r="BB11" s="43"/>
+      <c r="BC11" s="43"/>
+      <c r="BD11" s="43"/>
+      <c r="BE11" s="43"/>
+      <c r="BF11" s="43"/>
+      <c r="BG11" s="43"/>
+      <c r="BH11" s="43"/>
+      <c r="BI11" s="43"/>
+      <c r="BJ11" s="43"/>
+    </row>
+    <row r="12" spans="1:62" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="38">
+        <v>1</v>
+      </c>
+      <c r="D12" s="85">
+        <v>44957</v>
+      </c>
+      <c r="E12" s="85">
+        <v>44958</v>
+      </c>
+      <c r="F12" s="55">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="43"/>
+      <c r="Q12" s="43"/>
+      <c r="R12" s="43"/>
+      <c r="S12" s="43"/>
+      <c r="T12" s="43"/>
+      <c r="U12" s="43"/>
+      <c r="V12" s="43"/>
+      <c r="W12" s="43"/>
+      <c r="X12" s="43"/>
+      <c r="Y12" s="43"/>
+      <c r="Z12" s="43"/>
+      <c r="AA12" s="43"/>
+      <c r="AB12" s="43"/>
+      <c r="AC12" s="43"/>
+      <c r="AD12" s="43"/>
+      <c r="AE12" s="43"/>
+      <c r="AF12" s="43"/>
+      <c r="AG12" s="43"/>
+      <c r="AH12" s="43"/>
+      <c r="AI12" s="43"/>
+      <c r="AJ12" s="43"/>
+      <c r="AK12" s="43"/>
+      <c r="AL12" s="43"/>
+      <c r="AM12" s="43"/>
+      <c r="AN12" s="43"/>
+      <c r="AO12" s="43"/>
+      <c r="AP12" s="43"/>
+      <c r="AQ12" s="43"/>
+      <c r="AR12" s="43"/>
+      <c r="AS12" s="43"/>
+      <c r="AT12" s="43"/>
+      <c r="AU12" s="43"/>
+      <c r="AV12" s="43"/>
+      <c r="AW12" s="43"/>
+      <c r="AX12" s="43"/>
+      <c r="AY12" s="43"/>
+      <c r="AZ12" s="43"/>
+      <c r="BA12" s="43"/>
+      <c r="BB12" s="43"/>
+      <c r="BC12" s="43"/>
+      <c r="BD12" s="43"/>
+      <c r="BE12" s="43"/>
+      <c r="BF12" s="43"/>
+      <c r="BG12" s="43"/>
+      <c r="BH12" s="43"/>
+      <c r="BI12" s="43"/>
+      <c r="BJ12" s="43"/>
+    </row>
+    <row r="13" spans="1:62" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="38">
+        <v>1</v>
+      </c>
+      <c r="D13" s="85">
+        <v>44958</v>
+      </c>
+      <c r="E13" s="85">
+        <v>44959</v>
+      </c>
+      <c r="F13" s="55">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
+      <c r="K13" s="43"/>
+      <c r="L13" s="43"/>
+      <c r="M13" s="43"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
+      <c r="P13" s="43"/>
+      <c r="Q13" s="43"/>
+      <c r="R13" s="43"/>
+      <c r="S13" s="43"/>
+      <c r="T13" s="43"/>
+      <c r="U13" s="43"/>
+      <c r="V13" s="43"/>
+      <c r="W13" s="43"/>
+      <c r="X13" s="43"/>
+      <c r="Y13" s="43"/>
+      <c r="Z13" s="43"/>
+      <c r="AA13" s="43"/>
+      <c r="AB13" s="43"/>
+      <c r="AC13" s="43"/>
+      <c r="AD13" s="43"/>
+      <c r="AE13" s="43"/>
+      <c r="AF13" s="43"/>
+      <c r="AG13" s="43"/>
+      <c r="AH13" s="43"/>
+      <c r="AI13" s="43"/>
+      <c r="AJ13" s="43"/>
+      <c r="AK13" s="43"/>
+      <c r="AL13" s="43"/>
+      <c r="AM13" s="43"/>
+      <c r="AN13" s="43"/>
+      <c r="AO13" s="43"/>
+      <c r="AP13" s="43"/>
+      <c r="AQ13" s="43"/>
+      <c r="AR13" s="43"/>
+      <c r="AS13" s="43"/>
+      <c r="AT13" s="43"/>
+      <c r="AU13" s="43"/>
+      <c r="AV13" s="43"/>
+      <c r="AW13" s="43"/>
+      <c r="AX13" s="43"/>
+      <c r="AY13" s="43"/>
+      <c r="AZ13" s="43"/>
+      <c r="BA13" s="43"/>
+      <c r="BB13" s="43"/>
+      <c r="BC13" s="43"/>
+      <c r="BD13" s="43"/>
+      <c r="BE13" s="43"/>
+      <c r="BF13" s="43"/>
+      <c r="BG13" s="43"/>
+      <c r="BH13" s="43"/>
+      <c r="BI13" s="43"/>
+      <c r="BJ13" s="43"/>
+    </row>
+    <row r="14" spans="1:62" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="38">
+        <v>1</v>
+      </c>
+      <c r="D14" s="85">
+        <v>44959</v>
+      </c>
+      <c r="E14" s="85">
+        <v>44960</v>
+      </c>
+      <c r="F14" s="55">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="43"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="43"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="43"/>
+      <c r="T14" s="43"/>
+      <c r="U14" s="43"/>
+      <c r="V14" s="43"/>
+      <c r="W14" s="43"/>
+      <c r="X14" s="43"/>
+      <c r="Y14" s="43"/>
+      <c r="Z14" s="43"/>
+      <c r="AA14" s="43"/>
+      <c r="AB14" s="43"/>
+      <c r="AC14" s="43"/>
+      <c r="AD14" s="43"/>
+      <c r="AE14" s="43"/>
+      <c r="AF14" s="43"/>
+      <c r="AG14" s="43"/>
+      <c r="AH14" s="43"/>
+      <c r="AI14" s="43"/>
+      <c r="AJ14" s="43"/>
+      <c r="AK14" s="43"/>
+      <c r="AL14" s="43"/>
+      <c r="AM14" s="43"/>
+      <c r="AN14" s="43"/>
+      <c r="AO14" s="43"/>
+      <c r="AP14" s="43"/>
+      <c r="AQ14" s="43"/>
+      <c r="AR14" s="43"/>
+      <c r="AS14" s="43"/>
+      <c r="AT14" s="43"/>
+      <c r="AU14" s="43"/>
+      <c r="AV14" s="43"/>
+      <c r="AW14" s="43"/>
+      <c r="AX14" s="43"/>
+      <c r="AY14" s="43"/>
+      <c r="AZ14" s="43"/>
+      <c r="BA14" s="43"/>
+      <c r="BB14" s="43"/>
+      <c r="BC14" s="43"/>
+      <c r="BD14" s="43"/>
+      <c r="BE14" s="43"/>
+      <c r="BF14" s="43"/>
+      <c r="BG14" s="43"/>
+      <c r="BH14" s="43"/>
+      <c r="BI14" s="43"/>
+      <c r="BJ14" s="43"/>
+    </row>
+    <row r="15" spans="1:62" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="17"/>
+      <c r="B15" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="38">
+        <v>1</v>
+      </c>
+      <c r="D15" s="85">
+        <v>44960</v>
+      </c>
+      <c r="E15" s="85">
+        <v>44961</v>
+      </c>
+      <c r="F15" s="55">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="43"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="43"/>
+      <c r="P15" s="43"/>
+      <c r="Q15" s="43"/>
+      <c r="R15" s="43"/>
+      <c r="S15" s="43"/>
+      <c r="T15" s="43"/>
+      <c r="U15" s="43"/>
+      <c r="V15" s="43"/>
+      <c r="W15" s="43"/>
+      <c r="X15" s="43"/>
+      <c r="Y15" s="43"/>
+      <c r="Z15" s="43"/>
+      <c r="AA15" s="43"/>
+      <c r="AB15" s="43"/>
+      <c r="AC15" s="43"/>
+      <c r="AD15" s="43"/>
+      <c r="AE15" s="43"/>
+      <c r="AF15" s="43"/>
+      <c r="AG15" s="43"/>
+      <c r="AH15" s="43"/>
+      <c r="AI15" s="43"/>
+      <c r="AJ15" s="43"/>
+      <c r="AK15" s="43"/>
+      <c r="AL15" s="43"/>
+      <c r="AM15" s="43"/>
+      <c r="AN15" s="43"/>
+      <c r="AO15" s="43"/>
+      <c r="AP15" s="43"/>
+      <c r="AQ15" s="43"/>
+      <c r="AR15" s="43"/>
+      <c r="AS15" s="43"/>
+      <c r="AT15" s="43"/>
+      <c r="AU15" s="43"/>
+      <c r="AV15" s="43"/>
+      <c r="AW15" s="43"/>
+      <c r="AX15" s="43"/>
+      <c r="AY15" s="43"/>
+      <c r="AZ15" s="43"/>
+      <c r="BA15" s="43"/>
+      <c r="BB15" s="43"/>
+      <c r="BC15" s="43"/>
+      <c r="BD15" s="43"/>
+      <c r="BE15" s="43"/>
+      <c r="BF15" s="43"/>
+      <c r="BG15" s="43"/>
+      <c r="BH15" s="43"/>
+      <c r="BI15" s="43"/>
+      <c r="BJ15" s="43"/>
+    </row>
+    <row r="16" spans="1:62" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="40"/>
+      <c r="D16" s="75">
+        <v>44963</v>
+      </c>
+      <c r="E16" s="75">
+        <v>44969</v>
+      </c>
+      <c r="F16" s="76">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="43"/>
+      <c r="M16" s="43"/>
+      <c r="N16" s="43"/>
+      <c r="O16" s="43"/>
+      <c r="P16" s="43"/>
+      <c r="Q16" s="43"/>
+      <c r="R16" s="43"/>
+      <c r="S16" s="43"/>
+      <c r="T16" s="43"/>
+      <c r="U16" s="43"/>
+      <c r="V16" s="43"/>
+      <c r="W16" s="43"/>
+      <c r="X16" s="43"/>
+      <c r="Y16" s="43"/>
+      <c r="Z16" s="43"/>
+      <c r="AA16" s="43"/>
+      <c r="AB16" s="43"/>
+      <c r="AC16" s="43"/>
+      <c r="AD16" s="43"/>
+      <c r="AE16" s="43"/>
+      <c r="AF16" s="43"/>
+      <c r="AG16" s="43"/>
+      <c r="AH16" s="43"/>
+      <c r="AI16" s="43"/>
+      <c r="AJ16" s="43"/>
+      <c r="AK16" s="43"/>
+      <c r="AL16" s="43"/>
+      <c r="AM16" s="43"/>
+      <c r="AN16" s="43"/>
+      <c r="AO16" s="43"/>
+      <c r="AP16" s="43"/>
+      <c r="AQ16" s="43"/>
+      <c r="AR16" s="43"/>
+      <c r="AS16" s="43"/>
+      <c r="AT16" s="43"/>
+      <c r="AU16" s="43"/>
+      <c r="AV16" s="43"/>
+      <c r="AW16" s="43"/>
+      <c r="AX16" s="43"/>
+      <c r="AY16" s="43"/>
+      <c r="AZ16" s="43"/>
+      <c r="BA16" s="43"/>
+      <c r="BB16" s="43"/>
+      <c r="BC16" s="43"/>
+      <c r="BD16" s="43"/>
+      <c r="BE16" s="43"/>
+      <c r="BF16" s="43"/>
+      <c r="BG16" s="43"/>
+      <c r="BH16" s="43"/>
+      <c r="BI16" s="43"/>
+      <c r="BJ16" s="43"/>
+    </row>
+    <row r="17" spans="1:62" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="17"/>
+      <c r="B17" s="41" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="42">
+        <v>1</v>
+      </c>
+      <c r="D17" s="75">
+        <v>44963</v>
+      </c>
+      <c r="E17" s="75">
+        <v>44966</v>
+      </c>
+      <c r="F17" s="54">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="43"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="43"/>
+      <c r="O17" s="43"/>
+      <c r="P17" s="43"/>
+      <c r="Q17" s="43"/>
+      <c r="R17" s="43"/>
+      <c r="S17" s="43"/>
+      <c r="T17" s="43"/>
+      <c r="U17" s="43"/>
+      <c r="V17" s="43"/>
+      <c r="W17" s="44"/>
+      <c r="X17" s="43"/>
+      <c r="Y17" s="43"/>
+      <c r="Z17" s="43"/>
+      <c r="AA17" s="43"/>
+      <c r="AB17" s="43"/>
+      <c r="AC17" s="43"/>
+      <c r="AD17" s="43"/>
+      <c r="AE17" s="43"/>
+      <c r="AF17" s="43"/>
+      <c r="AG17" s="43"/>
+      <c r="AH17" s="43"/>
+      <c r="AI17" s="43"/>
+      <c r="AJ17" s="43"/>
+      <c r="AK17" s="43"/>
+      <c r="AL17" s="43"/>
+      <c r="AM17" s="43"/>
+      <c r="AN17" s="43"/>
+      <c r="AO17" s="43"/>
+      <c r="AP17" s="43"/>
+      <c r="AQ17" s="43"/>
+      <c r="AR17" s="43"/>
+      <c r="AS17" s="43"/>
+      <c r="AT17" s="43"/>
+      <c r="AU17" s="43"/>
+      <c r="AV17" s="43"/>
+      <c r="AW17" s="43"/>
+      <c r="AX17" s="43"/>
+      <c r="AY17" s="43"/>
+      <c r="AZ17" s="43"/>
+      <c r="BA17" s="43"/>
+      <c r="BB17" s="43"/>
+      <c r="BC17" s="43"/>
+      <c r="BD17" s="43"/>
+      <c r="BE17" s="43"/>
+      <c r="BF17" s="43"/>
+      <c r="BG17" s="43"/>
+      <c r="BH17" s="43"/>
+      <c r="BI17" s="43"/>
+      <c r="BJ17" s="43"/>
+    </row>
+    <row r="18" spans="1:62" s="2" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="17"/>
+      <c r="B18" s="41" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="42">
+        <v>1</v>
+      </c>
+      <c r="D18" s="75">
+        <v>44967</v>
+      </c>
+      <c r="E18" s="75">
+        <v>44969</v>
+      </c>
+      <c r="F18" s="54">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="G18" s="92"/>
+      <c r="H18" s="92"/>
+      <c r="I18" s="92"/>
+      <c r="J18" s="92"/>
+      <c r="K18" s="92"/>
+      <c r="L18" s="92"/>
+      <c r="M18" s="92"/>
+      <c r="N18" s="92"/>
+      <c r="O18" s="92"/>
+      <c r="P18" s="92"/>
+      <c r="Q18" s="92"/>
+      <c r="R18" s="92"/>
+      <c r="S18" s="92"/>
+      <c r="T18" s="92"/>
+      <c r="U18" s="92"/>
+      <c r="V18" s="92"/>
+      <c r="W18" s="93"/>
+      <c r="X18" s="92"/>
+      <c r="Y18" s="92"/>
+      <c r="Z18" s="92"/>
+      <c r="AA18" s="92"/>
+      <c r="AB18" s="92"/>
+      <c r="AC18" s="92"/>
+      <c r="AD18" s="92"/>
+      <c r="AE18" s="92"/>
+      <c r="AF18" s="92"/>
+      <c r="AG18" s="92"/>
+      <c r="AH18" s="92"/>
+      <c r="AI18" s="92"/>
+      <c r="AJ18" s="92"/>
+      <c r="AK18" s="92"/>
+      <c r="AL18" s="92"/>
+      <c r="AM18" s="92"/>
+      <c r="AN18" s="92"/>
+      <c r="AO18" s="92"/>
+      <c r="AP18" s="92"/>
+      <c r="AQ18" s="92"/>
+      <c r="AR18" s="92"/>
+      <c r="AS18" s="92"/>
+      <c r="AT18" s="92"/>
+      <c r="AU18" s="92"/>
+      <c r="AV18" s="92"/>
+      <c r="AW18" s="92"/>
+      <c r="AX18" s="92"/>
+      <c r="AY18" s="92"/>
+      <c r="AZ18" s="92"/>
+      <c r="BA18" s="92"/>
+      <c r="BB18" s="92"/>
+      <c r="BC18" s="92"/>
+      <c r="BD18" s="92"/>
+      <c r="BE18" s="92"/>
+      <c r="BF18" s="92"/>
+      <c r="BG18" s="92"/>
+      <c r="BH18" s="92"/>
+      <c r="BI18" s="92"/>
+      <c r="BJ18" s="92"/>
+    </row>
+    <row r="19" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+    </row>
+    <row r="20" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="B20" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="47">
+        <v>43113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="B21" s="50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="B22" s="49" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="AB4:AH4"/>
+    <mergeCell ref="AI4:AO4"/>
+    <mergeCell ref="AP4:AV4"/>
+    <mergeCell ref="AW4:BC4"/>
+    <mergeCell ref="BD4:BJ4"/>
+    <mergeCell ref="H1:Y1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G4:M4"/>
+    <mergeCell ref="N4:T4"/>
+    <mergeCell ref="U4:AA4"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C7:C18">
+    <cfRule type="dataBar" priority="31">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="2" tint="-0.499984740745262"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{9E9D36D1-B10F-474B-BF30-56FCA3B38051}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G7:BJ18">
+    <cfRule type="expression" dxfId="2" priority="32">
+      <formula>AND(task_start&lt;=G$5,ROUNDDOWN((task_end-task_start+1)*task_progress,0)+task_start-1&gt;=G$5)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="33" stopIfTrue="1">
+      <formula>AND(task_end&gt;=G$5,task_start&lt;G$5+1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5:BJ18">
+    <cfRule type="expression" dxfId="0" priority="34">
+      <formula>AND(today&gt;=G$5,today&lt;G$5+1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Changing this number will scroll the Gantt Chart view." sqref="D4" xr:uid="{32DDAB17-9BF6-4711-A73A-D6DFEE5CBD18}">
+      <formula1>1</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B21" r:id="rId1" xr:uid="{CD4A2419-AC75-45A8-B49B-29A009FAFD33}"/>
+    <hyperlink ref="B20" r:id="rId2" xr:uid="{3C66C4FC-110F-497B-B908-17698314ABB7}"/>
+  </hyperlinks>
+  <pageMargins left="0.35" right="0.35" top="0.35" bottom="0.5" header="0.3" footer="0.3"/>
+  <pageSetup scale="58" fitToHeight="0" orientation="landscape" r:id="rId3"/>
+  <headerFooter scaleWithDoc="0"/>
+  <legacyDrawing r:id="rId4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{9E9D36D1-B10F-474B-BF30-56FCA3B38051}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C7:C18</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>